<commit_message>
new modifications and test of automatically transforms text
</commit_message>
<xml_diff>
--- a/original-datasets/FS_01_DOWN_ANNOT.xlsx
+++ b/original-datasets/FS_01_DOWN_ANNOT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\COMPARACIONES ANOT Y ENRIQUECIMIENTO\COLORES\FS_01_DOWN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises Olivares\Dropbox\19. GitHub\Merge-Genomic-Data\original-datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,8 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5744,7 +5743,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5825,8 +5824,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6107,7 +6134,7 @@
       <selection activeCell="F1079" sqref="F1079"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>

</xml_diff>